<commit_message>
cap nhat den ctdt
</commit_message>
<xml_diff>
--- a/data/CTDT/CTDT IT1.xlsx
+++ b/data/CTDT/CTDT IT1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tài liệu học tập\2024.2\Cơ sở dữ liệu_IT3292\Thực hành\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\BTL_DB_2024\data\CTDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC24FCF3-3483-4CD1-ADCE-414BA73EA267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994D495F-AA49-4110-B268-3F0CD63F0ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="408" yWindow="2664" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="261">
   <si>
     <t>IT4995</t>
   </si>
@@ -784,9 +784,6 @@
   </si>
   <si>
     <t>TC học</t>
-  </si>
-  <si>
-    <t>Mã HP học</t>
   </si>
   <si>
     <t>Ghi chú loại HP</t>
@@ -916,7 +913,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -928,7 +925,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
@@ -1211,34 +1207,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M112"/>
+  <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="56.5703125" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="8" width="13.5546875" customWidth="1"/>
+    <col min="9" max="9" width="56.5546875" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>247</v>
@@ -1267,3414 +1262,2852 @@
       <c r="K1" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="B2" s="5" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2">
         <v>8</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5">
+      <c r="G2">
         <v>6</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>210</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5">
-        <v>2</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5">
-        <v>2</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5" t="s">
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>210</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="5">
-        <v>3</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5">
-        <v>3</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>210</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5">
-        <v>2</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5" t="s">
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6" t="s">
+      <c r="L5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>210</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5">
-        <v>2</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5" t="s">
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="6" t="s">
+      <c r="L6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>210</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7">
         <v>6</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5">
-        <v>2</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5" t="s">
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="6" t="s">
+      <c r="L7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>210</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8">
         <v>7</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5">
-        <v>2</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5" t="s">
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="6" t="s">
+      <c r="L8" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>220</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="6" t="s">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>220</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="6" t="s">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>220</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="5">
-        <v>2</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="6" t="s">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>220</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="5">
-        <v>3</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="6" t="s">
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>220</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13">
         <v>4</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="6" t="s">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>220</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14">
         <v>5</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="6" t="s">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>220</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="5">
-        <v>3</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="6" t="s">
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>220</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="5">
-        <v>3</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="6" t="s">
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>220</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17">
         <v>4</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="6" t="s">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>220</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18">
         <v>5</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="6" t="s">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>220</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="5">
-        <v>3</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5">
-        <v>0</v>
-      </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="6" t="s">
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>220</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20">
         <v>4</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5">
-        <v>0</v>
-      </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="6" t="s">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>220</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21">
         <v>5</v>
       </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="6" t="s">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>220</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="5">
-        <v>3</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5">
-        <v>0</v>
-      </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="6" t="s">
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>220</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="5">
-        <v>3</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5">
-        <v>0</v>
-      </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="6" t="s">
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>220</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5">
-        <v>0</v>
-      </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="6" t="s">
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>220</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25">
         <v>5</v>
       </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5">
-        <v>0</v>
-      </c>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="6" t="s">
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>220</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="5">
-        <v>3</v>
-      </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5">
-        <v>0</v>
-      </c>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="6" t="s">
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>220</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27">
         <v>4</v>
       </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5">
-        <v>0</v>
-      </c>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="6" t="s">
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>220</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28">
         <v>5</v>
       </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5">
-        <v>0</v>
-      </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="6" t="s">
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>220</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" t="s">
         <v>21</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="5">
-        <v>3</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="6" t="s">
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>220</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30">
         <v>4</v>
       </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5">
-        <v>0</v>
-      </c>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="6" t="s">
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>220</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" t="s">
         <v>21</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31">
         <v>5</v>
       </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5">
-        <v>0</v>
-      </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="6" t="s">
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>220</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" t="s">
         <v>21</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5">
-        <v>0</v>
-      </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="6" t="s">
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>220</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" t="s">
         <v>21</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" t="s">
         <v>71</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" t="s">
         <v>69</v>
       </c>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5">
-        <v>0</v>
-      </c>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="6" t="s">
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>220</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" t="s">
         <v>21</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" t="s">
         <v>73</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" t="s">
         <v>69</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5">
-        <v>0</v>
-      </c>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="6" t="s">
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>220</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" t="s">
         <v>21</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" t="s">
         <v>69</v>
       </c>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5">
-        <v>0</v>
-      </c>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="6" t="s">
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>220</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" t="s">
         <v>21</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36">
         <v>1</v>
       </c>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5">
-        <v>0</v>
-      </c>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="6" t="s">
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>220</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="5">
-        <v>2</v>
-      </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5">
-        <v>0</v>
-      </c>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="6" t="s">
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>220</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" t="s">
         <v>21</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" t="s">
         <v>81</v>
       </c>
-      <c r="E38" s="5">
-        <v>3</v>
-      </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5">
-        <v>0</v>
-      </c>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="6" t="s">
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>21</v>
+      </c>
+      <c r="L38" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>220</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" t="s">
         <v>21</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" t="s">
         <v>83</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39">
         <v>4</v>
       </c>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5">
-        <v>0</v>
-      </c>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="6" t="s">
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>21</v>
+      </c>
+      <c r="L39" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>220</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" t="s">
         <v>21</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" t="s">
         <v>85</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40">
         <v>5</v>
       </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5">
-        <v>0</v>
-      </c>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="6" t="s">
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>21</v>
+      </c>
+      <c r="L40" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>220</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" t="s">
         <v>21</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" t="s">
         <v>87</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5">
-        <v>0</v>
-      </c>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="6" t="s">
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
+        <v>21</v>
+      </c>
+      <c r="L41" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:12">
       <c r="A42">
         <v>220</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" t="s">
         <v>21</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" t="s">
         <v>89</v>
       </c>
-      <c r="E42" s="5">
-        <v>2</v>
-      </c>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5">
-        <v>0</v>
-      </c>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="6" t="s">
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>21</v>
+      </c>
+      <c r="L42" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:12">
       <c r="A43">
         <v>220</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" t="s">
         <v>21</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" t="s">
         <v>91</v>
       </c>
-      <c r="E43" s="5">
-        <v>3</v>
-      </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5">
-        <v>0</v>
-      </c>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="6" t="s">
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>21</v>
+      </c>
+      <c r="L43" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>220</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" t="s">
         <v>21</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44">
         <v>4</v>
       </c>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5">
-        <v>0</v>
-      </c>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="6" t="s">
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="I44" t="s">
+        <v>21</v>
+      </c>
+      <c r="L44" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>220</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" t="s">
         <v>95</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45">
         <v>5</v>
       </c>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5">
-        <v>0</v>
-      </c>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="6" t="s">
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>21</v>
+      </c>
+      <c r="L45" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:12">
       <c r="A46">
         <v>220</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" t="s">
         <v>21</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" t="s">
         <v>97</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46">
         <v>1</v>
       </c>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5">
-        <v>0</v>
-      </c>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="6" t="s">
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>21</v>
+      </c>
+      <c r="L46" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:12">
       <c r="A47">
         <v>220</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" t="s">
         <v>21</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" t="s">
         <v>99</v>
       </c>
-      <c r="E47" s="5">
-        <v>2</v>
-      </c>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5">
-        <v>0</v>
-      </c>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="6" t="s">
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L47" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:12">
       <c r="A48">
         <v>220</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" t="s">
         <v>21</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" t="s">
         <v>101</v>
       </c>
-      <c r="E48" s="5">
-        <v>3</v>
-      </c>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5">
-        <v>0</v>
-      </c>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="6" t="s">
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>21</v>
+      </c>
+      <c r="L48" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:12">
       <c r="A49">
         <v>220</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" t="s">
         <v>21</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" t="s">
         <v>103</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49">
         <v>4</v>
       </c>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5">
-        <v>0</v>
-      </c>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="6" t="s">
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>21</v>
+      </c>
+      <c r="L49" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:12">
       <c r="A50">
         <v>220</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" t="s">
         <v>21</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" t="s">
         <v>105</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50">
         <v>5</v>
       </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5">
-        <v>0</v>
-      </c>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="6" t="s">
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="I50" t="s">
+        <v>21</v>
+      </c>
+      <c r="L50" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:12">
       <c r="A51">
         <v>230</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" t="s">
         <v>108</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" t="s">
         <v>107</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51">
         <v>1</v>
       </c>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5">
-        <v>0</v>
-      </c>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5" t="s">
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
         <v>108</v>
       </c>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="6" t="s">
+      <c r="L51" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:12">
       <c r="A52">
         <v>230</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" t="s">
         <v>108</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" t="s">
         <v>111</v>
       </c>
-      <c r="E52" s="5">
-        <v>2</v>
-      </c>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5">
-        <v>0</v>
-      </c>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5" t="s">
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
         <v>108</v>
       </c>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="6" t="s">
+      <c r="L52" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:12">
       <c r="A53">
         <v>230</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" t="s">
         <v>108</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" t="s">
         <v>113</v>
       </c>
-      <c r="E53" s="5">
-        <v>2</v>
-      </c>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5">
-        <v>0</v>
-      </c>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5" t="s">
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
         <v>108</v>
       </c>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="6" t="s">
+      <c r="L53" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:12">
       <c r="A54">
         <v>230</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" t="s">
         <v>108</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" t="s">
         <v>115</v>
       </c>
-      <c r="E54" s="5">
-        <v>2</v>
-      </c>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5">
-        <v>0</v>
-      </c>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5" t="s">
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
         <v>108</v>
       </c>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="6" t="s">
+      <c r="L54" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:12">
       <c r="A55">
         <v>241</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" t="s">
         <v>118</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" t="s">
         <v>117</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55">
         <v>1</v>
       </c>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5">
-        <v>0</v>
-      </c>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5" t="s">
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
         <v>118</v>
       </c>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="6" t="s">
+      <c r="L55" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:12">
       <c r="A56">
         <v>241</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" t="s">
         <v>118</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" t="s">
         <v>121</v>
       </c>
-      <c r="E56" s="5">
-        <v>2</v>
-      </c>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5">
-        <v>0</v>
-      </c>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5" t="s">
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
         <v>118</v>
       </c>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="6" t="s">
+      <c r="L56" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:12">
       <c r="A57">
         <v>250</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" t="s">
         <v>124</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" t="s">
         <v>123</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E57">
         <v>1</v>
       </c>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5">
+      <c r="G57">
         <v>4</v>
       </c>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5" t="s">
+      <c r="I57" t="s">
         <v>124</v>
       </c>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
-      <c r="M57" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="L57" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58">
         <v>250</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" t="s">
         <v>124</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" t="s">
         <v>126</v>
       </c>
-      <c r="E58" s="5">
-        <v>2</v>
-      </c>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5">
-        <v>3</v>
-      </c>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="5" t="s">
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="I58" t="s">
         <v>124</v>
       </c>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
-      <c r="M58" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="L58" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59">
         <v>250</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" t="s">
         <v>124</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" t="s">
         <v>128</v>
       </c>
-      <c r="E59" s="5">
+      <c r="E59">
         <v>1</v>
       </c>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5">
+      <c r="G59">
         <v>4</v>
       </c>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="5" t="s">
+      <c r="I59" t="s">
         <v>124</v>
       </c>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-      <c r="M59" s="6" t="s">
+      <c r="L59" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:12">
       <c r="A60">
         <v>250</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" t="s">
         <v>124</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" t="s">
         <v>131</v>
       </c>
-      <c r="E60" s="5">
-        <v>2</v>
-      </c>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5">
-        <v>3</v>
-      </c>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5" t="s">
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+      <c r="I60" t="s">
         <v>124</v>
       </c>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
-      <c r="M60" s="6" t="s">
+      <c r="L60" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:12">
       <c r="A61">
         <v>250</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" t="s">
         <v>124</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" t="s">
         <v>133</v>
       </c>
-      <c r="E61" s="5">
-        <v>3</v>
-      </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5">
-        <v>3</v>
-      </c>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5" t="s">
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+      <c r="I61" t="s">
         <v>124</v>
       </c>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-      <c r="M61" s="6" t="s">
+      <c r="L61" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:12">
       <c r="A62">
         <v>250</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" t="s">
         <v>124</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" t="s">
         <v>135</v>
       </c>
-      <c r="E62" s="5">
+      <c r="E62">
         <v>1</v>
       </c>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5">
+      <c r="G62">
         <v>4</v>
       </c>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5" t="s">
+      <c r="I62" t="s">
         <v>124</v>
       </c>
-      <c r="K62" s="5"/>
-      <c r="L62" s="5"/>
-      <c r="M62" s="6" t="s">
+      <c r="L62" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:12">
       <c r="A63">
         <v>250</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" t="s">
         <v>124</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" t="s">
         <v>137</v>
       </c>
-      <c r="E63" s="5">
-        <v>3</v>
-      </c>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5">
-        <v>3</v>
-      </c>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5" t="s">
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>3</v>
+      </c>
+      <c r="I63" t="s">
         <v>124</v>
       </c>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
-      <c r="M63" s="6" t="s">
+      <c r="L63" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:12">
       <c r="A64">
         <v>250</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" t="s">
         <v>124</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" t="s">
         <v>139</v>
       </c>
-      <c r="E64" s="5">
-        <v>3</v>
-      </c>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5">
-        <v>2</v>
-      </c>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5" t="s">
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="G64">
+        <v>2</v>
+      </c>
+      <c r="I64" t="s">
         <v>124</v>
       </c>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="6" t="s">
+      <c r="L64" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:12">
       <c r="A65">
         <v>250</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" t="s">
         <v>124</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" t="s">
         <v>141</v>
       </c>
-      <c r="E65" s="5">
-        <v>2</v>
-      </c>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5">
-        <v>3</v>
-      </c>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5" t="s">
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="G65">
+        <v>3</v>
+      </c>
+      <c r="I65" t="s">
         <v>124</v>
       </c>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
-      <c r="M65" s="6" t="s">
+      <c r="L65" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:12">
       <c r="A66">
         <v>250</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" t="s">
         <v>124</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" t="s">
         <v>144</v>
       </c>
-      <c r="E66" s="5">
-        <v>3</v>
-      </c>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5">
-        <v>3</v>
-      </c>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5" t="s">
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="G66">
+        <v>3</v>
+      </c>
+      <c r="I66" t="s">
         <v>124</v>
       </c>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5"/>
-      <c r="M66" s="6" t="s">
+      <c r="L66" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:12">
       <c r="A67">
         <v>300</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" t="s">
         <v>147</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" t="s">
         <v>146</v>
       </c>
-      <c r="E67" s="5">
+      <c r="E67">
         <v>1</v>
       </c>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5">
-        <v>3</v>
-      </c>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5" t="s">
+      <c r="G67">
+        <v>3</v>
+      </c>
+      <c r="I67" t="s">
         <v>147</v>
       </c>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="L67" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68">
         <v>300</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" t="s">
         <v>147</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" t="s">
         <v>149</v>
       </c>
-      <c r="E68" s="5">
-        <v>2</v>
-      </c>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5">
-        <v>2</v>
-      </c>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5" t="s">
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="G68">
+        <v>2</v>
+      </c>
+      <c r="I68" t="s">
         <v>147</v>
       </c>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
-      <c r="M68" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="L68" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69">
         <v>300</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" t="s">
         <v>147</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" t="s">
         <v>151</v>
       </c>
-      <c r="E69" s="5">
-        <v>3</v>
-      </c>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5">
-        <v>3</v>
-      </c>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5" t="s">
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="G69">
+        <v>3</v>
+      </c>
+      <c r="I69" t="s">
         <v>147</v>
       </c>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="L69" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70">
         <v>300</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" t="s">
         <v>147</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" t="s">
         <v>153</v>
       </c>
-      <c r="E70" s="5">
+      <c r="E70">
         <v>4</v>
       </c>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5">
-        <v>2</v>
-      </c>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5" t="s">
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="I70" t="s">
         <v>147</v>
       </c>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="L70" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71">
         <v>300</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" t="s">
         <v>147</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" t="s">
         <v>155</v>
       </c>
-      <c r="E71" s="5">
+      <c r="E71">
         <v>4</v>
       </c>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5">
-        <v>3</v>
-      </c>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5" t="s">
+      <c r="G71">
+        <v>3</v>
+      </c>
+      <c r="I71" t="s">
         <v>147</v>
       </c>
-      <c r="K71" s="5"/>
-      <c r="L71" s="5"/>
-      <c r="M71" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="L71" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72">
         <v>300</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" t="s">
         <v>147</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" t="s">
         <v>157</v>
       </c>
-      <c r="E72" s="5">
+      <c r="E72">
         <v>4</v>
       </c>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5">
-        <v>3</v>
-      </c>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
-      <c r="J72" s="5" t="s">
+      <c r="G72">
+        <v>3</v>
+      </c>
+      <c r="I72" t="s">
         <v>147</v>
       </c>
-      <c r="K72" s="5"/>
-      <c r="L72" s="5"/>
-      <c r="M72" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="L72" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73">
         <v>300</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" t="s">
         <v>147</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" t="s">
         <v>159</v>
       </c>
-      <c r="E73" s="5">
+      <c r="E73">
         <v>5</v>
       </c>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5">
-        <v>3</v>
-      </c>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5" t="s">
+      <c r="G73">
+        <v>3</v>
+      </c>
+      <c r="I73" t="s">
         <v>147</v>
       </c>
-      <c r="K73" s="5"/>
-      <c r="L73" s="5"/>
-      <c r="M73" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="L73" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74">
         <v>300</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" t="s">
         <v>147</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" t="s">
         <v>161</v>
       </c>
-      <c r="E74" s="5">
-        <v>3</v>
-      </c>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5">
-        <v>2</v>
-      </c>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5" t="s">
+      <c r="E74">
+        <v>3</v>
+      </c>
+      <c r="G74">
+        <v>2</v>
+      </c>
+      <c r="I74" t="s">
         <v>147</v>
       </c>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="L74" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75">
         <v>300</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" t="s">
         <v>147</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" t="s">
         <v>163</v>
       </c>
-      <c r="E75" s="5">
+      <c r="E75">
         <v>6</v>
       </c>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5">
-        <v>2</v>
-      </c>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5" t="s">
+      <c r="G75">
+        <v>2</v>
+      </c>
+      <c r="I75" t="s">
         <v>147</v>
       </c>
-      <c r="K75" s="5"/>
-      <c r="L75" s="5"/>
-      <c r="M75" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="L75" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76">
         <v>300</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" t="s">
         <v>147</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" t="s">
         <v>165</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E76">
         <v>5</v>
       </c>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5">
-        <v>2</v>
-      </c>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
-      <c r="J76" s="5" t="s">
+      <c r="G76">
+        <v>2</v>
+      </c>
+      <c r="I76" t="s">
         <v>147</v>
       </c>
-      <c r="K76" s="5"/>
-      <c r="L76" s="5"/>
-      <c r="M76" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="L76" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77">
         <v>300</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" t="s">
         <v>147</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" t="s">
         <v>167</v>
       </c>
-      <c r="E77" s="5">
+      <c r="E77">
         <v>4</v>
       </c>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5">
-        <v>3</v>
-      </c>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
-      <c r="J77" s="5" t="s">
+      <c r="G77">
+        <v>3</v>
+      </c>
+      <c r="I77" t="s">
         <v>147</v>
       </c>
-      <c r="K77" s="5"/>
-      <c r="L77" s="5"/>
-      <c r="M77" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="L77" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78">
         <v>300</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" t="s">
         <v>147</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" t="s">
         <v>169</v>
       </c>
-      <c r="E78" s="5">
+      <c r="E78">
         <v>5</v>
       </c>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5">
-        <v>2</v>
-      </c>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
-      <c r="J78" s="5" t="s">
+      <c r="G78">
+        <v>2</v>
+      </c>
+      <c r="I78" t="s">
         <v>147</v>
       </c>
-      <c r="K78" s="5"/>
-      <c r="L78" s="5"/>
-      <c r="M78" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="L78" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79">
         <v>300</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" t="s">
         <v>147</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" t="s">
         <v>171</v>
       </c>
-      <c r="E79" s="5">
+      <c r="E79">
         <v>5</v>
       </c>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5">
-        <v>3</v>
-      </c>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
-      <c r="J79" s="5" t="s">
+      <c r="G79">
+        <v>3</v>
+      </c>
+      <c r="I79" t="s">
         <v>147</v>
       </c>
-      <c r="K79" s="5"/>
-      <c r="L79" s="5"/>
-      <c r="M79" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="L79" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80">
         <v>300</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" t="s">
         <v>147</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" t="s">
         <v>173</v>
       </c>
-      <c r="E80" s="5">
+      <c r="E80">
         <v>5</v>
       </c>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5">
-        <v>3</v>
-      </c>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
-      <c r="J80" s="5" t="s">
+      <c r="G80">
+        <v>3</v>
+      </c>
+      <c r="I80" t="s">
         <v>147</v>
       </c>
-      <c r="K80" s="5"/>
-      <c r="L80" s="5"/>
-      <c r="M80" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="L80" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81">
         <v>300</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" t="s">
         <v>147</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" t="s">
         <v>175</v>
       </c>
-      <c r="E81" s="5">
+      <c r="E81">
         <v>6</v>
       </c>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5">
-        <v>2</v>
-      </c>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
-      <c r="J81" s="5" t="s">
+      <c r="G81">
+        <v>2</v>
+      </c>
+      <c r="I81" t="s">
         <v>147</v>
       </c>
-      <c r="K81" s="5"/>
-      <c r="L81" s="5"/>
-      <c r="M81" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="L81" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82">
         <v>300</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" t="s">
         <v>147</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" t="s">
         <v>177</v>
       </c>
-      <c r="E82" s="5">
+      <c r="E82">
         <v>7</v>
       </c>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5">
-        <v>3</v>
-      </c>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
-      <c r="J82" s="5" t="s">
+      <c r="G82">
+        <v>3</v>
+      </c>
+      <c r="I82" t="s">
         <v>147</v>
       </c>
-      <c r="K82" s="5"/>
-      <c r="L82" s="5"/>
-      <c r="M82" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="L82" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83">
         <v>300</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" t="s">
         <v>147</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" t="s">
         <v>179</v>
       </c>
-      <c r="E83" s="5">
+      <c r="E83">
         <v>6</v>
       </c>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5">
-        <v>3</v>
-      </c>
-      <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
-      <c r="J83" s="5" t="s">
+      <c r="G83">
+        <v>3</v>
+      </c>
+      <c r="I83" t="s">
         <v>147</v>
       </c>
-      <c r="K83" s="5"/>
-      <c r="L83" s="5"/>
-      <c r="M83" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="L83" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84">
         <v>300</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" t="s">
         <v>147</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" t="s">
         <v>181</v>
       </c>
-      <c r="E84" s="5">
+      <c r="E84">
         <v>8</v>
       </c>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5">
-        <v>2</v>
-      </c>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
-      <c r="J84" s="5" t="s">
+      <c r="G84">
+        <v>2</v>
+      </c>
+      <c r="I84" t="s">
         <v>147</v>
       </c>
-      <c r="K84" s="5"/>
-      <c r="L84" s="5"/>
-      <c r="M84" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="L84" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85">
         <v>300</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" t="s">
         <v>147</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" t="s">
         <v>183</v>
       </c>
-      <c r="E85" s="5">
+      <c r="E85">
         <v>6</v>
       </c>
-      <c r="F85" s="5"/>
-      <c r="G85" s="5">
-        <v>2</v>
-      </c>
-      <c r="H85" s="5"/>
-      <c r="I85" s="5"/>
-      <c r="J85" s="5" t="s">
+      <c r="G85">
+        <v>2</v>
+      </c>
+      <c r="I85" t="s">
         <v>147</v>
       </c>
-      <c r="K85" s="5"/>
-      <c r="L85" s="5"/>
-      <c r="M85" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13">
+      <c r="L85" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86">
         <v>320</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" t="s">
         <v>186</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" t="s">
         <v>185</v>
       </c>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="5">
-        <v>2</v>
-      </c>
-      <c r="H86" s="5"/>
-      <c r="I86" s="5"/>
-      <c r="J86" s="5" t="s">
+      <c r="G86">
+        <v>2</v>
+      </c>
+      <c r="I86" t="s">
         <v>186</v>
       </c>
-      <c r="K86" s="5"/>
-      <c r="L86" s="5"/>
-      <c r="M86" s="6" t="s">
+      <c r="L86" s="5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:12">
       <c r="A87">
         <v>320</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" t="s">
         <v>186</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" t="s">
         <v>189</v>
       </c>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="5">
-        <v>2</v>
-      </c>
-      <c r="H87" s="5"/>
-      <c r="I87" s="5"/>
-      <c r="J87" s="5" t="s">
+      <c r="G87">
+        <v>2</v>
+      </c>
+      <c r="I87" t="s">
         <v>186</v>
       </c>
-      <c r="K87" s="5"/>
-      <c r="L87" s="5"/>
-      <c r="M87" s="6" t="s">
+      <c r="L87" s="5" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:12">
       <c r="A88">
         <v>320</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" t="s">
         <v>186</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" t="s">
         <v>192</v>
       </c>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="5">
-        <v>2</v>
-      </c>
-      <c r="H88" s="5"/>
-      <c r="I88" s="5"/>
-      <c r="J88" s="5" t="s">
+      <c r="G88">
+        <v>2</v>
+      </c>
+      <c r="I88" t="s">
         <v>186</v>
       </c>
-      <c r="K88" s="5"/>
-      <c r="L88" s="5"/>
-      <c r="M88" s="6" t="s">
+      <c r="L88" s="5" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:12">
       <c r="A89">
         <v>320</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" t="s">
         <v>186</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" t="s">
         <v>194</v>
       </c>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="5">
-        <v>2</v>
-      </c>
-      <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
-      <c r="J89" s="5" t="s">
+      <c r="G89">
+        <v>2</v>
+      </c>
+      <c r="I89" t="s">
         <v>186</v>
       </c>
-      <c r="K89" s="5"/>
-      <c r="L89" s="5"/>
-      <c r="M89" s="6" t="s">
+      <c r="L89" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:12">
       <c r="A90">
         <v>320</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" t="s">
         <v>186</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" t="s">
         <v>196</v>
       </c>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5">
-        <v>2</v>
-      </c>
-      <c r="H90" s="5"/>
-      <c r="I90" s="5"/>
-      <c r="J90" s="5" t="s">
+      <c r="G90">
+        <v>2</v>
+      </c>
+      <c r="I90" t="s">
         <v>186</v>
       </c>
-      <c r="K90" s="5"/>
-      <c r="L90" s="5"/>
-      <c r="M90" s="6" t="s">
+      <c r="L90" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:12">
       <c r="A91">
         <v>320</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" t="s">
         <v>186</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" t="s">
         <v>198</v>
       </c>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5">
-        <v>2</v>
-      </c>
-      <c r="H91" s="5"/>
-      <c r="I91" s="5"/>
-      <c r="J91" s="5" t="s">
+      <c r="G91">
+        <v>2</v>
+      </c>
+      <c r="I91" t="s">
         <v>186</v>
       </c>
-      <c r="K91" s="5"/>
-      <c r="L91" s="5"/>
-      <c r="M91" s="6" t="s">
+      <c r="L91" s="5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:12">
       <c r="A92">
         <v>320</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" t="s">
         <v>186</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D92" t="s">
         <v>201</v>
       </c>
-      <c r="E92" s="5">
+      <c r="E92">
         <v>4</v>
       </c>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5">
-        <v>3</v>
-      </c>
-      <c r="H92" s="5"/>
-      <c r="I92" s="5"/>
-      <c r="J92" s="5" t="s">
+      <c r="G92">
+        <v>3</v>
+      </c>
+      <c r="I92" t="s">
         <v>186</v>
       </c>
-      <c r="K92" s="5"/>
-      <c r="L92" s="5"/>
-      <c r="M92" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13">
+      <c r="L92" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93">
         <v>320</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" t="s">
         <v>186</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D93" t="s">
         <v>203</v>
       </c>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="5">
-        <v>2</v>
-      </c>
-      <c r="H93" s="5"/>
-      <c r="I93" s="5"/>
-      <c r="J93" s="5" t="s">
+      <c r="G93">
+        <v>2</v>
+      </c>
+      <c r="I93" t="s">
         <v>186</v>
       </c>
-      <c r="K93" s="5"/>
-      <c r="L93" s="5"/>
-      <c r="M93" s="6" t="s">
+      <c r="L93" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:12">
       <c r="A94">
         <v>320</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" t="s">
         <v>186</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" t="s">
         <v>206</v>
       </c>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5">
-        <v>2</v>
-      </c>
-      <c r="H94" s="5"/>
-      <c r="I94" s="5"/>
-      <c r="J94" s="5" t="s">
+      <c r="G94">
+        <v>2</v>
+      </c>
+      <c r="I94" t="s">
         <v>186</v>
       </c>
-      <c r="K94" s="5"/>
-      <c r="L94" s="5"/>
-      <c r="M94" s="6" t="s">
+      <c r="L94" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:12">
       <c r="A95">
         <v>320</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" t="s">
         <v>186</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" t="s">
         <v>203</v>
       </c>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5">
-        <v>2</v>
-      </c>
-      <c r="H95" s="5"/>
-      <c r="I95" s="5"/>
-      <c r="J95" s="5" t="s">
+      <c r="G95">
+        <v>2</v>
+      </c>
+      <c r="I95" t="s">
         <v>186</v>
       </c>
-      <c r="K95" s="5"/>
-      <c r="L95" s="5"/>
-      <c r="M95" s="6" t="s">
+      <c r="L95" s="5" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:12">
       <c r="A96">
         <v>360</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" t="s">
         <v>211</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" t="s">
         <v>210</v>
       </c>
-      <c r="E96" s="5">
+      <c r="E96">
         <v>6</v>
       </c>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5">
-        <v>2</v>
-      </c>
-      <c r="H96" s="5"/>
-      <c r="I96" s="5"/>
-      <c r="J96" s="5" t="s">
+      <c r="G96">
+        <v>2</v>
+      </c>
+      <c r="I96" t="s">
         <v>211</v>
       </c>
-      <c r="K96" s="5"/>
-      <c r="L96" s="5"/>
-      <c r="M96" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13">
+      <c r="L96" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
       <c r="A97">
         <v>400</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" t="s">
         <v>214</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" t="s">
         <v>213</v>
       </c>
-      <c r="E97" s="5">
+      <c r="E97">
         <v>7</v>
       </c>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5">
-        <v>3</v>
-      </c>
-      <c r="H97" s="5"/>
-      <c r="I97" s="5"/>
-      <c r="J97" s="5" t="s">
+      <c r="G97">
+        <v>3</v>
+      </c>
+      <c r="I97" t="s">
         <v>214</v>
       </c>
-      <c r="K97" s="5"/>
-      <c r="L97" s="5"/>
-      <c r="M97" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="L97" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98">
         <v>400</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" t="s">
         <v>214</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D98" t="s">
         <v>216</v>
       </c>
-      <c r="E98" s="5">
+      <c r="E98">
         <v>7</v>
       </c>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5">
-        <v>3</v>
-      </c>
-      <c r="H98" s="5"/>
-      <c r="I98" s="5"/>
-      <c r="J98" s="5" t="s">
+      <c r="G98">
+        <v>3</v>
+      </c>
+      <c r="I98" t="s">
         <v>214</v>
       </c>
-      <c r="K98" s="5"/>
-      <c r="L98" s="5"/>
-      <c r="M98" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13">
+      <c r="L98" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99">
         <v>400</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" t="s">
         <v>214</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" t="s">
         <v>218</v>
       </c>
-      <c r="E99" s="5">
+      <c r="E99">
         <v>7</v>
       </c>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5">
-        <v>2</v>
-      </c>
-      <c r="H99" s="5"/>
-      <c r="I99" s="5"/>
-      <c r="J99" s="5" t="s">
+      <c r="G99">
+        <v>2</v>
+      </c>
+      <c r="I99" t="s">
         <v>214</v>
       </c>
-      <c r="K99" s="5"/>
-      <c r="L99" s="5"/>
-      <c r="M99" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13">
+      <c r="L99" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
       <c r="A100">
         <v>400</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" t="s">
         <v>214</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D100" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E100" s="5">
+      <c r="D100" t="s">
+        <v>220</v>
+      </c>
+      <c r="E100">
         <v>7</v>
       </c>
-      <c r="F100" s="5"/>
-      <c r="G100" s="5">
-        <v>2</v>
-      </c>
-      <c r="H100" s="5"/>
-      <c r="I100" s="5"/>
-      <c r="J100" s="5" t="s">
+      <c r="G100">
+        <v>2</v>
+      </c>
+      <c r="I100" t="s">
         <v>214</v>
       </c>
-      <c r="K100" s="5"/>
-      <c r="L100" s="5"/>
-      <c r="M100" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13">
+      <c r="L100" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101">
         <v>401</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" t="s">
         <v>223</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" t="s">
         <v>222</v>
       </c>
-      <c r="E101" s="5">
+      <c r="E101">
         <v>7</v>
       </c>
-      <c r="F101" s="5"/>
-      <c r="G101" s="5">
-        <v>2</v>
-      </c>
-      <c r="H101" s="5"/>
-      <c r="I101" s="5"/>
-      <c r="J101" s="5" t="s">
+      <c r="G101">
+        <v>2</v>
+      </c>
+      <c r="I101" t="s">
         <v>223</v>
       </c>
-      <c r="K101" s="5"/>
-      <c r="L101" s="5"/>
-      <c r="M101" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13">
+      <c r="L101" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
       <c r="A102">
         <v>401</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" t="s">
         <v>223</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" t="s">
         <v>225</v>
       </c>
-      <c r="E102" s="5">
+      <c r="E102">
         <v>7</v>
       </c>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5">
-        <v>3</v>
-      </c>
-      <c r="H102" s="5"/>
-      <c r="I102" s="5"/>
-      <c r="J102" s="5" t="s">
+      <c r="G102">
+        <v>3</v>
+      </c>
+      <c r="I102" t="s">
         <v>223</v>
       </c>
-      <c r="K102" s="5"/>
-      <c r="L102" s="5"/>
-      <c r="M102" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13">
+      <c r="L102" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103">
         <v>401</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" t="s">
         <v>223</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" t="s">
         <v>227</v>
       </c>
-      <c r="E103" s="5">
+      <c r="E103">
         <v>7</v>
       </c>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5">
-        <v>2</v>
-      </c>
-      <c r="H103" s="5"/>
-      <c r="I103" s="5"/>
-      <c r="J103" s="5" t="s">
+      <c r="G103">
+        <v>2</v>
+      </c>
+      <c r="I103" t="s">
         <v>223</v>
       </c>
-      <c r="K103" s="5"/>
-      <c r="L103" s="5"/>
-      <c r="M103" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13">
+      <c r="L103" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104">
         <v>401</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" t="s">
         <v>223</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D104" s="5" t="s">
+      <c r="D104" t="s">
         <v>229</v>
       </c>
-      <c r="E104" s="5">
+      <c r="E104">
         <v>7</v>
       </c>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5">
-        <v>3</v>
-      </c>
-      <c r="H104" s="5"/>
-      <c r="I104" s="5"/>
-      <c r="J104" s="5" t="s">
+      <c r="G104">
+        <v>3</v>
+      </c>
+      <c r="I104" t="s">
         <v>223</v>
       </c>
-      <c r="K104" s="5"/>
-      <c r="L104" s="5"/>
-      <c r="M104" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13">
+      <c r="L104" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105">
         <v>402</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" t="s">
         <v>232</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="D105" t="s">
         <v>231</v>
       </c>
-      <c r="E105" s="5">
+      <c r="E105">
         <v>7</v>
       </c>
-      <c r="F105" s="5"/>
-      <c r="G105" s="5">
-        <v>3</v>
-      </c>
-      <c r="H105" s="5"/>
-      <c r="I105" s="5"/>
-      <c r="J105" s="5" t="s">
+      <c r="G105">
+        <v>3</v>
+      </c>
+      <c r="I105" t="s">
         <v>232</v>
       </c>
-      <c r="K105" s="5"/>
-      <c r="L105" s="5"/>
-      <c r="M105" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13">
+      <c r="L105" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
       <c r="A106">
         <v>402</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" t="s">
         <v>232</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D106" s="5" t="s">
+      <c r="D106" t="s">
         <v>234</v>
       </c>
-      <c r="E106" s="5">
+      <c r="E106">
         <v>7</v>
       </c>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5">
-        <v>2</v>
-      </c>
-      <c r="H106" s="5"/>
-      <c r="I106" s="5"/>
-      <c r="J106" s="5" t="s">
+      <c r="G106">
+        <v>2</v>
+      </c>
+      <c r="I106" t="s">
         <v>232</v>
       </c>
-      <c r="K106" s="5"/>
-      <c r="L106" s="5"/>
-      <c r="M106" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13">
+      <c r="L106" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
       <c r="A107">
         <v>402</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" t="s">
         <v>232</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="D107" s="5" t="s">
+      <c r="D107" t="s">
         <v>236</v>
       </c>
-      <c r="E107" s="5">
+      <c r="E107">
         <v>7</v>
       </c>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5">
-        <v>3</v>
-      </c>
-      <c r="H107" s="5"/>
-      <c r="I107" s="5"/>
-      <c r="J107" s="5" t="s">
+      <c r="G107">
+        <v>3</v>
+      </c>
+      <c r="I107" t="s">
         <v>232</v>
       </c>
-      <c r="K107" s="5"/>
-      <c r="L107" s="5"/>
-      <c r="M107" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13">
+      <c r="L107" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
       <c r="A108">
         <v>402</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" t="s">
         <v>232</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D108" s="5" t="s">
+      <c r="D108" t="s">
         <v>238</v>
       </c>
-      <c r="E108" s="5">
+      <c r="E108">
         <v>7</v>
       </c>
-      <c r="F108" s="5"/>
-      <c r="G108" s="5">
-        <v>2</v>
-      </c>
-      <c r="H108" s="5"/>
-      <c r="I108" s="5"/>
-      <c r="J108" s="5" t="s">
+      <c r="G108">
+        <v>2</v>
+      </c>
+      <c r="I108" t="s">
         <v>232</v>
       </c>
-      <c r="K108" s="5"/>
-      <c r="L108" s="5"/>
-      <c r="M108" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13">
+      <c r="L108" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109">
         <v>403</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B109" t="s">
         <v>241</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="D109" t="s">
         <v>240</v>
       </c>
-      <c r="E109" s="5">
+      <c r="E109">
         <v>6</v>
       </c>
-      <c r="F109" s="5"/>
-      <c r="G109" s="5">
-        <v>3</v>
-      </c>
-      <c r="H109" s="5"/>
-      <c r="I109" s="5"/>
-      <c r="J109" s="5" t="s">
+      <c r="G109">
+        <v>3</v>
+      </c>
+      <c r="I109" t="s">
         <v>241</v>
       </c>
-      <c r="K109" s="5"/>
-      <c r="L109" s="5"/>
-      <c r="M109" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13">
+      <c r="L109" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
       <c r="A110">
         <v>403</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B110" t="s">
         <v>241</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="D110" s="5" t="s">
+      <c r="D110" t="s">
         <v>243</v>
       </c>
-      <c r="E110" s="5">
+      <c r="E110">
         <v>7</v>
       </c>
-      <c r="F110" s="5"/>
-      <c r="G110" s="5">
-        <v>3</v>
-      </c>
-      <c r="H110" s="5"/>
-      <c r="I110" s="5"/>
-      <c r="J110" s="5" t="s">
+      <c r="G110">
+        <v>3</v>
+      </c>
+      <c r="I110" t="s">
         <v>241</v>
       </c>
-      <c r="K110" s="5"/>
-      <c r="L110" s="5"/>
-      <c r="M110" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13">
+      <c r="L110" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
       <c r="A111">
         <v>404</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B111" t="s">
         <v>246</v>
       </c>
-      <c r="C111" s="5" t="s">
+      <c r="C111" t="s">
         <v>244</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="D111" t="s">
         <v>245</v>
       </c>
-      <c r="E111" s="5">
+      <c r="E111">
         <v>7</v>
       </c>
-      <c r="F111" s="5"/>
-      <c r="G111" s="5">
-        <v>3</v>
-      </c>
-      <c r="H111" s="5"/>
-      <c r="I111" s="5"/>
-      <c r="J111" s="5" t="s">
+      <c r="G111">
+        <v>3</v>
+      </c>
+      <c r="I111" t="s">
         <v>246</v>
       </c>
-      <c r="K111" s="5"/>
-      <c r="L111" s="5"/>
-      <c r="M111" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13">
+      <c r="L111" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
       <c r="A112">
         <v>404</v>
       </c>
-      <c r="B112" s="7" t="s">
+      <c r="B112" s="6" t="s">
         <v>246</v>
       </c>
       <c r="C112" t="s">
+        <v>259</v>
+      </c>
+      <c r="D112" t="s">
         <v>260</v>
-      </c>
-      <c r="D112" t="s">
-        <v>261</v>
       </c>
       <c r="E112">
         <v>6</v>
@@ -4682,7 +4115,7 @@
       <c r="G112">
         <v>3</v>
       </c>
-      <c r="J112" s="5" t="s">
+      <c r="I112" t="s">
         <v>246</v>
       </c>
     </row>

</xml_diff>